<commit_message>
[code comitted on 23 nov 2025]
</commit_message>
<xml_diff>
--- a/src/main/resources/TestDATA.xlsx
+++ b/src/main/resources/TestDATA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Employee Name</t>
   </si>
@@ -41,6 +41,37 @@
   </si>
   <si>
     <t xml:space="preserve">Jobin 
+</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>Katrina</t>
+  </si>
+  <si>
+    <t>Kaif</t>
+  </si>
+  <si>
+    <t>Kareena</t>
+  </si>
+  <si>
+    <t>Kapoor</t>
+  </si>
+  <si>
+    <t>Rahul Dravid</t>
+  </si>
+  <si>
+    <t>12@misty@12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joele mathew
 </t>
   </si>
 </sst>
@@ -77,12 +108,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -365,46 +397,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3">
+        <v>8677</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3">
+        <v>8678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>